<commit_message>
revise markingresult to list
</commit_message>
<xml_diff>
--- a/data/答案.xlsx
+++ b/data/答案.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
     <t>题号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -27,35 +27,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>分值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -63,7 +35,16 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ABD</t>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -427,7 +408,7 @@
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -447,10 +428,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -458,10 +439,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1">
-        <v>5</v>
+        <v>8.33</v>
       </c>
       <c r="D2" s="1">
         <v>1.5</v>
@@ -472,10 +453,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1">
-        <v>5</v>
+        <v>8.33</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -486,10 +467,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1">
-        <v>5</v>
+        <v>8.33</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
@@ -500,10 +481,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1">
-        <v>5</v>
+        <v>8.33</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -514,10 +495,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1">
-        <v>5</v>
+        <v>8.33</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
@@ -528,10 +509,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1">
-        <v>5</v>
+        <v>8.33</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
@@ -542,10 +523,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1">
-        <v>5</v>
+        <v>8.33</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
@@ -556,10 +537,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1">
-        <v>5</v>
+        <v>8.33</v>
       </c>
       <c r="D9" s="1">
         <v>0</v>
@@ -569,15 +550,8 @@
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1">
-        <v>5</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -587,7 +561,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="1">
-        <v>5</v>
+        <v>8.33</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
@@ -598,10 +572,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C12" s="1">
-        <v>5</v>
+        <v>8.33</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
@@ -615,16 +589,25 @@
         <v>4</v>
       </c>
       <c r="C13" s="1">
-        <v>5</v>
+        <v>8.33</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="1"/>
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="1">
+        <v>8.33</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>

</xml_diff>